<commit_message>
Few changes and UserUnitTest
</commit_message>
<xml_diff>
--- a/public/FIN13Inicial.xlsx
+++ b/public/FIN13Inicial.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="35">
   <si>
     <t>PLAN OPERATIVO DE GRUPOS Y SEMILLEROS DE INVESTIGACIÓN</t>
   </si>
@@ -36,7 +36,7 @@
     <t>DIRECTOR DEL GRUPO Y/O SEMILLERO</t>
   </si>
   <si>
-    <t>José Alejandro Cortés Taborda</t>
+    <t>Jose Alejandro Cortés Taborda</t>
   </si>
   <si>
     <t>SEMESTRE</t>
@@ -87,22 +87,7 @@
     <t>aula</t>
   </si>
   <si>
-    <t>X</t>
-  </si>
-  <si>
     <t>FH05</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> prueba 1 prueba 2</t>
-  </si>
-  <si>
-    <t>Segunda</t>
-  </si>
-  <si>
-    <t>Estudiante</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> prueba 3</t>
   </si>
   <si>
     <t xml:space="preserve">HORARIO DE REUNIÓN: </t>
@@ -129,16 +114,10 @@
     <t>EMAIL</t>
   </si>
   <si>
-    <t>Maicol Duque Urrea</t>
+    <t>Director</t>
   </si>
   <si>
-    <t>maicol_duque82141@elpoli.edu.co</t>
-  </si>
-  <si>
-    <t>Brayan Legarda Villegas</t>
-  </si>
-  <si>
-    <t>brayan_legarda82132@elpoli.edu.co</t>
+    <t>jose_cortes82141@elpoli.edu.co</t>
   </si>
   <si>
     <r>
@@ -1004,21 +983,15 @@
       <c r="C10" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>23</v>
-      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
       <c r="I10" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
-      <c r="J10" s="10" t="s">
-        <v>25</v>
-      </c>
+      <c r="J10" s="10"/>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
       <c r="M10" s="5"/>
@@ -1100,30 +1073,16 @@
       <c r="CK10" s="5"/>
     </row>
     <row r="11" spans="1:89" customHeight="1" ht="15" s="1" customFormat="1">
-      <c r="A11" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>22</v>
-      </c>
+      <c r="A11" s="10"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
-      <c r="F11" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>23</v>
-      </c>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
       <c r="H11" s="4"/>
-      <c r="I11" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="J11" s="10" t="s">
-        <v>28</v>
-      </c>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
       <c r="M11" s="5"/>
@@ -1779,7 +1738,7 @@
     </row>
     <row r="21" spans="1:89" customHeight="1" ht="18.75">
       <c r="A21" s="9" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -3213,7 +3172,7 @@
       <c r="C1" s="17"/>
       <c r="D1" s="17"/>
       <c r="E1" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
@@ -3346,7 +3305,7 @@
     </row>
     <row r="4" spans="1:45" customHeight="1" ht="15">
       <c r="A4" s="18" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B4" s="18"/>
       <c r="C4" s="18"/>
@@ -3355,54 +3314,44 @@
     </row>
     <row r="5" spans="1:45" customHeight="1" ht="38.25">
       <c r="A5" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:45" customHeight="1" ht="15">
+      <c r="A6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="C6" s="7">
+        <v>1035</v>
+      </c>
+      <c r="D6" s="7">
+        <v>12</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:45" customHeight="1" ht="15">
-      <c r="A6" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="7">
-        <v>121312321</v>
-      </c>
-      <c r="D6" s="7">
-        <v>30523124</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>38</v>
-      </c>
     </row>
     <row r="7" spans="1:45" customHeight="1" ht="15">
-      <c r="A7" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="7">
-        <v>56156</v>
-      </c>
-      <c r="D7" s="7">
-        <v>30231321934</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>40</v>
-      </c>
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
     </row>
     <row r="8" spans="1:45" customHeight="1" ht="15">
       <c r="A8" s="7"/>
@@ -3632,7 +3581,7 @@
     </row>
     <row r="18" spans="1:45" customHeight="1" ht="15">
       <c r="A18" s="3" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B18" s="3"/>
     </row>

</xml_diff>